<commit_message>
Added option to list existing sources/sinks for virtual_nodes.py
</commit_message>
<xml_diff>
--- a/data/simple_pd_network_no_virtual_virtual.xlsx
+++ b/data/simple_pd_network_no_virtual_virtual.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -811,7 +811,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>clearance_0</t>
+          <t>cma_0</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -836,7 +836,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>cma_0</t>
+          <t>gba_0</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -861,7 +861,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>gba_0</t>
+          <t>glucose_0</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -886,7 +886,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>glucose_0</t>
+          <t>lrrk2_0</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -911,7 +911,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>lrrk2_0</t>
+          <t>mutant_a_syn_0</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -936,7 +936,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>mutant_a_syn_0</t>
+          <t>mutant_lrrk2_0</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -961,7 +961,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>mutant_lrrk2_0</t>
+          <t>scarb2_0</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -986,12 +986,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>scarb2_0</t>
+          <t>s0</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>e10</t>
+          <t>a_syn_0</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1011,12 +1011,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>s0</t>
+          <t>s1</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>a_syn_0</t>
+          <t>glucosylceramide_0</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1036,12 +1036,12 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>s1</t>
+          <t>s2</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>glucosylceramide_0</t>
+          <t>lamp2_0</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1061,12 +1061,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>s2</t>
+          <t>s3</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>lamp2_0</t>
+          <t>lrrk2_0</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1086,12 +1086,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>s3</t>
+          <t>s4</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>lrrk2_0</t>
+          <t>mis_a_syn_0</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1111,12 +1111,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>s4</t>
+          <t>s5</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>mis_a_syn_0</t>
+          <t>mutant_a_syn_0</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1136,12 +1136,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>s5</t>
+          <t>s6</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>mutant_a_syn_0</t>
+          <t>mutant_lrrk2_0</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1161,12 +1161,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>s6</t>
+          <t>s7</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>mutant_lrrk2_0</t>
+          <t>scarb2_gba_golgi_0</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1175,31 +1175,6 @@
         </is>
       </c>
       <c r="E30" t="inlineStr">
-        <is>
-          <t>none</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="1" t="n">
-        <v>29</v>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>s7</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>scarb2_gba_golgi_0</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>none</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
         <is>
           <t>none</t>
         </is>

</xml_diff>